<commit_message>
this is a third commit
</commit_message>
<xml_diff>
--- a/testdata/Opencart_LoginData.xlsx
+++ b/testdata/Opencart_LoginData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7EC1B0EB-D8A9-44B9-8051-341AAFB506E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{850E732F-C36C-47C6-B8EB-6C0FCD92735E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
   </bookViews>
@@ -15,15 +15,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -183,10 +174,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -510,7 +501,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>